<commit_message>
add sound for button and door
</commit_message>
<xml_diff>
--- a/RoomTracking.xlsx
+++ b/RoomTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\Avem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F84F0E6-8AAE-4A07-A061-D0611F00A0A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870FC745-DB0B-4398-BB67-FA63274F94D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>LvLDesign</t>
   </si>
@@ -283,6 +283,18 @@
   </si>
   <si>
     <t>our face</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>RoomSasTransition</t>
+  </si>
+  <si>
+    <t>RoomSas</t>
+  </si>
+  <si>
+    <t>RoomExit</t>
   </si>
 </sst>
 </file>
@@ -777,7 +789,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -891,6 +903,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -1177,8 +1199,8 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L37" sqref="L37"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,11 +2133,11 @@
       <c r="B49" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
+      <c r="G49" s="22"/>
       <c r="H49" s="27"/>
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
@@ -2183,28 +2205,72 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
-      <c r="L53" s="6"/>
-      <c r="M53" s="45"/>
+      <c r="A53" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="26"/>
+      <c r="K53" s="26"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="32"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="56"/>
+      <c r="B54" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="58"/>
+      <c r="F54" s="58"/>
+      <c r="G54" s="58"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
+      <c r="K54" s="58"/>
+      <c r="L54" s="58"/>
       <c r="M54" s="33"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M55" s="33"/>
+    <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="57"/>
+      <c r="B55" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="27"/>
+      <c r="M55" s="34"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M56" s="33"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="45"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M57" s="33"/>
@@ -2234,6 +2300,9 @@
       <c r="M66" s="33"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A53:A55"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add etail and the last room lvldesign
</commit_message>
<xml_diff>
--- a/RoomTracking.xlsx
+++ b/RoomTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\Avem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870FC745-DB0B-4398-BB67-FA63274F94D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BC499-BD58-479A-8C03-9BF0056A039C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -903,6 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,7 +913,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
@@ -1199,8 +1199,8 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,10 +2121,10 @@
       <c r="E48" s="21"/>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
-      <c r="H48" s="26"/>
+      <c r="H48" s="21"/>
       <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
       <c r="L48" s="26"/>
       <c r="M48" s="32"/>
     </row>
@@ -2138,10 +2138,10 @@
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
       <c r="G49" s="22"/>
-      <c r="H49" s="27"/>
+      <c r="H49" s="22"/>
       <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
       <c r="L49" s="27"/>
       <c r="M49" s="34"/>
     </row>
@@ -2205,7 +2205,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="55" t="s">
+      <c r="A53" s="56" t="s">
         <v>86</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -2213,47 +2213,47 @@
       </c>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
       <c r="I53" s="26"/>
       <c r="J53" s="26"/>
-      <c r="K53" s="26"/>
+      <c r="K53" s="21"/>
       <c r="L53" s="26"/>
       <c r="M53" s="32"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
+      <c r="A54" s="57"/>
       <c r="B54" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="24"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="58"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="55"/>
+      <c r="J54" s="55"/>
+      <c r="K54" s="24"/>
+      <c r="L54" s="55"/>
       <c r="M54" s="33"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="57"/>
+      <c r="A55" s="58"/>
       <c r="B55" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="27"/>
-      <c r="K55" s="27"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
       <c r="L55" s="27"/>
       <c r="M55" s="34"/>
     </row>

</xml_diff>

<commit_message>
add light to the last lvl
</commit_message>
<xml_diff>
--- a/RoomTracking.xlsx
+++ b/RoomTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\Avem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962BC499-BD58-479A-8C03-9BF0056A039C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E38359-8AB9-47D3-A572-15E18FAE40B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="91">
   <si>
     <t>LvLDesign</t>
   </si>
@@ -295,13 +295,16 @@
   </si>
   <si>
     <t>RoomExit</t>
+  </si>
+  <si>
+    <t>RoomPassage1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,20 +321,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,11 +337,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -783,13 +774,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -828,22 +818,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -876,9 +864,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -892,7 +877,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -903,7 +888,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -914,9 +898,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutre" xfId="3" builtinId="28"/>
+  <cellStyles count="3">
+    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -1199,8 +1182,8 @@
   <dimension ref="A1:T66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,54 +1204,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-    </row>
-    <row r="2" spans="1:20" s="54" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+    </row>
+    <row r="2" spans="1:20" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
@@ -1285,7 +1268,7 @@
       <c r="J2" s="20"/>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
-      <c r="M2" s="29"/>
+      <c r="M2" s="27"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -1311,7 +1294,7 @@
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
-      <c r="M3" s="30"/>
+      <c r="M3" s="28"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -1328,7 +1311,7 @@
       <c r="J4" s="22"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
-      <c r="M4" s="31"/>
+      <c r="M4" s="29"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -1347,7 +1330,7 @@
       <c r="J5" s="21"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
-      <c r="M5" s="32"/>
+      <c r="M5" s="30"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
@@ -1364,7 +1347,7 @@
       <c r="J6" s="24"/>
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
-      <c r="M6" s="33"/>
+      <c r="M6" s="31"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
@@ -1381,7 +1364,7 @@
       <c r="J7" s="24"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
-      <c r="M7" s="33"/>
+      <c r="M7" s="31"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
@@ -1398,7 +1381,7 @@
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
-      <c r="M8" s="33"/>
+      <c r="M8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
@@ -1415,7 +1398,7 @@
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
-      <c r="M9" s="33"/>
+      <c r="M9" s="31"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
@@ -1432,7 +1415,7 @@
       <c r="J10" s="24"/>
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
-      <c r="M10" s="33"/>
+      <c r="M10" s="31"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
@@ -1449,7 +1432,7 @@
       <c r="J11" s="24"/>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="33"/>
+      <c r="M11" s="31"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
@@ -1466,7 +1449,7 @@
       <c r="J12" s="24"/>
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
-      <c r="M12" s="33"/>
+      <c r="M12" s="31"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
@@ -1483,7 +1466,7 @@
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
       <c r="L13" s="22"/>
-      <c r="M13" s="34"/>
+      <c r="M13" s="32"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1502,7 +1485,7 @@
       <c r="J14" s="21"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="35" t="s">
+      <c r="M14" s="33" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1521,7 +1504,7 @@
       <c r="J15" s="22"/>
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="36"/>
+      <c r="M15" s="34"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1540,7 +1523,7 @@
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
-      <c r="M16" s="37">
+      <c r="M16" s="35">
         <v>11</v>
       </c>
     </row>
@@ -1559,7 +1542,7 @@
       <c r="J17" s="25"/>
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
-      <c r="M17" s="38" t="s">
+      <c r="M17" s="36" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1580,7 +1563,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="21"/>
-      <c r="M18" s="32"/>
+      <c r="M18" s="30"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
@@ -1597,7 +1580,7 @@
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
-      <c r="M19" s="33"/>
+      <c r="M19" s="31"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
@@ -1614,7 +1597,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
-      <c r="M20" s="33"/>
+      <c r="M20" s="31"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
@@ -1631,7 +1614,7 @@
       <c r="J21" s="24"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
-      <c r="M21" s="33"/>
+      <c r="M21" s="31"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
@@ -1648,7 +1631,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
-      <c r="M22" s="33"/>
+      <c r="M22" s="31"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
@@ -1665,7 +1648,7 @@
       <c r="J23" s="24"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
-      <c r="M23" s="39">
+      <c r="M23" s="37">
         <v>17</v>
       </c>
     </row>
@@ -1684,7 +1667,7 @@
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
-      <c r="M24" s="33"/>
+      <c r="M24" s="31"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
@@ -1701,7 +1684,7 @@
       <c r="J25" s="24"/>
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
-      <c r="M25" s="39">
+      <c r="M25" s="37">
         <v>11</v>
       </c>
     </row>
@@ -1720,7 +1703,7 @@
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
-      <c r="M26" s="34"/>
+      <c r="M26" s="32"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -1739,7 +1722,7 @@
       <c r="J27" s="21"/>
       <c r="K27" s="21"/>
       <c r="L27" s="21"/>
-      <c r="M27" s="40"/>
+      <c r="M27" s="38"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
@@ -1756,7 +1739,7 @@
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
-      <c r="M28" s="41" t="s">
+      <c r="M28" s="39" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1777,7 +1760,7 @@
       <c r="J29" s="20"/>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
-      <c r="M29" s="46" t="s">
+      <c r="M29" s="43" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1788,17 +1771,17 @@
       <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="48"/>
-      <c r="M30" s="49">
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="46">
         <v>14</v>
       </c>
     </row>
@@ -1813,11 +1796,11 @@
       <c r="F31" s="24"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
-      <c r="I31" s="48"/>
+      <c r="I31" s="45"/>
       <c r="J31" s="24"/>
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
-      <c r="M31" s="39">
+      <c r="M31" s="37">
         <v>6</v>
       </c>
     </row>
@@ -1836,7 +1819,7 @@
       <c r="J32" s="24"/>
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
-      <c r="M32" s="39" t="s">
+      <c r="M32" s="37" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1855,7 +1838,7 @@
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
-      <c r="M33" s="33"/>
+      <c r="M33" s="31"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
@@ -1872,7 +1855,7 @@
       <c r="J34" s="24"/>
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
-      <c r="M34" s="42">
+      <c r="M34" s="37">
         <v>12</v>
       </c>
     </row>
@@ -1891,7 +1874,7 @@
       <c r="J35" s="24"/>
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
-      <c r="M35" s="47"/>
+      <c r="M35" s="44"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
@@ -1908,7 +1891,7 @@
       <c r="J36" s="24"/>
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
-      <c r="M36" s="39">
+      <c r="M36" s="37">
         <v>23</v>
       </c>
     </row>
@@ -1927,7 +1910,7 @@
       <c r="J37" s="24"/>
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
-      <c r="M37" s="33"/>
+      <c r="M37" s="31"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
@@ -1944,7 +1927,7 @@
       <c r="J38" s="22"/>
       <c r="K38" s="22"/>
       <c r="L38" s="22"/>
-      <c r="M38" s="34"/>
+      <c r="M38" s="32"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -1963,7 +1946,7 @@
       <c r="J39" s="21"/>
       <c r="K39" s="21"/>
       <c r="L39" s="21"/>
-      <c r="M39" s="32"/>
+      <c r="M39" s="30"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
@@ -1980,7 +1963,7 @@
       <c r="J40" s="22"/>
       <c r="K40" s="22"/>
       <c r="L40" s="22"/>
-      <c r="M40" s="34"/>
+      <c r="M40" s="32"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
@@ -1989,17 +1972,17 @@
       <c r="B41" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="43"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="40"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
@@ -2018,7 +2001,7 @@
       <c r="J42" s="20"/>
       <c r="K42" s="20"/>
       <c r="L42" s="20"/>
-      <c r="M42" s="44"/>
+      <c r="M42" s="41"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -2037,7 +2020,7 @@
       <c r="J43" s="21"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
-      <c r="M43" s="32"/>
+      <c r="M43" s="30"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
@@ -2054,7 +2037,7 @@
       <c r="J44" s="24"/>
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
-      <c r="M44" s="33"/>
+      <c r="M44" s="31"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
@@ -2071,7 +2054,7 @@
       <c r="J45" s="24"/>
       <c r="K45" s="24"/>
       <c r="L45" s="24"/>
-      <c r="M45" s="33"/>
+      <c r="M45" s="31"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
@@ -2088,7 +2071,7 @@
       <c r="J46" s="22"/>
       <c r="K46" s="22"/>
       <c r="L46" s="22"/>
-      <c r="M46" s="34"/>
+      <c r="M46" s="32"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
@@ -2097,17 +2080,17 @@
       <c r="B47" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="28"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="28"/>
-      <c r="M47" s="43"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="40"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
@@ -2122,28 +2105,28 @@
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
-      <c r="I48" s="26"/>
+      <c r="I48" s="21"/>
       <c r="J48" s="21"/>
       <c r="K48" s="21"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="32"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="30"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C49" s="22"/>
       <c r="D49" s="22"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="22"/>
       <c r="H49" s="22"/>
-      <c r="I49" s="27"/>
+      <c r="I49" s="22"/>
       <c r="J49" s="22"/>
       <c r="K49" s="22"/>
-      <c r="L49" s="27"/>
-      <c r="M49" s="34"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="32"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -2157,12 +2140,12 @@
       <c r="E50" s="21"/>
       <c r="F50" s="21"/>
       <c r="G50" s="21"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="32"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="30"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
@@ -2179,7 +2162,7 @@
       <c r="J51" s="22"/>
       <c r="K51" s="22"/>
       <c r="L51" s="22"/>
-      <c r="M51" s="41" t="s">
+      <c r="M51" s="39" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2200,12 +2183,12 @@
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
       <c r="L52" s="20"/>
-      <c r="M52" s="46" t="s">
+      <c r="M52" s="43" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="56" t="s">
+      <c r="A53" s="52" t="s">
         <v>86</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -2217,14 +2200,14 @@
       <c r="F53" s="21"/>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="26"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
       <c r="K53" s="21"/>
-      <c r="L53" s="26"/>
-      <c r="M53" s="32"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="30"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="57"/>
+      <c r="A54" s="53"/>
       <c r="B54" s="3" t="s">
         <v>88</v>
       </c>
@@ -2234,14 +2217,14 @@
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
       <c r="H54" s="24"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="55"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
       <c r="K54" s="24"/>
-      <c r="L54" s="55"/>
-      <c r="M54" s="33"/>
+      <c r="L54" s="24"/>
+      <c r="M54" s="31"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="58"/>
+      <c r="A55" s="54"/>
       <c r="B55" s="14" t="s">
         <v>89</v>
       </c>
@@ -2254,8 +2237,8 @@
       <c r="I55" s="22"/>
       <c r="J55" s="22"/>
       <c r="K55" s="22"/>
-      <c r="L55" s="27"/>
-      <c r="M55" s="34"/>
+      <c r="L55" s="22"/>
+      <c r="M55" s="32"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
@@ -2270,34 +2253,34 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="45"/>
+      <c r="M56" s="42"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M57" s="33"/>
+      <c r="M57" s="31"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M58" s="33"/>
+      <c r="M58" s="31"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M59" s="33"/>
+      <c r="M59" s="31"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M60" s="33"/>
+      <c r="M60" s="31"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M61" s="33"/>
+      <c r="M61" s="31"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M62" s="33"/>
+      <c r="M62" s="31"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M63" s="33"/>
+      <c r="M63" s="31"/>
     </row>
     <row r="65" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M65" s="33"/>
+      <c r="M65" s="31"/>
     </row>
     <row r="66" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M66" s="33"/>
+      <c r="M66" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
make final check on the wall
</commit_message>
<xml_diff>
--- a/RoomTracking.xlsx
+++ b/RoomTracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GameMaking\Avem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E38359-8AB9-47D3-A572-15E18FAE40B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB0E786-45B7-4D67-94A5-2F014787B3C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="480" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,15 +319,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,11 +334,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -774,10 +762,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -818,20 +805,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -877,7 +857,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -897,9 +876,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Neutre" xfId="2" builtinId="28"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
@@ -1183,7 +1169,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,71 +1190,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-    </row>
-    <row r="2" spans="1:20" s="51" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+    </row>
+    <row r="2" spans="1:20" s="43" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="27"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="20"/>
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
@@ -1284,34 +1270,34 @@
       <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="28"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="21"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="29"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
@@ -1320,153 +1306,153 @@
       <c r="B5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="30"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="31"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="31"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="24"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="31"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="31"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="24"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="31"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="31"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="24"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="31"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="32"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -1475,17 +1461,17 @@
       <c r="B14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="33" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="26" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1494,17 +1480,17 @@
       <c r="B15" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="34"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="27"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1513,17 +1499,17 @@
       <c r="B16" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="35">
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="28">
         <v>11</v>
       </c>
     </row>
@@ -1532,17 +1518,17 @@
       <c r="B17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="36" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="29" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1553,102 +1539,102 @@
       <c r="B18" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="30"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="23"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="31"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="24"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="31"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="31"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="24"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="31"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="37">
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="30">
         <v>17</v>
       </c>
     </row>
@@ -1657,34 +1643,34 @@
       <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="31"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="24"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="37">
+      <c r="C25" s="51"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="51"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
+      <c r="M25" s="30">
         <v>11</v>
       </c>
     </row>
@@ -1693,17 +1679,17 @@
       <c r="B26" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="32"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
@@ -1712,34 +1698,34 @@
       <c r="B27" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="38"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="31"/>
     </row>
     <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="39" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="32" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1750,17 +1736,17 @@
       <c r="B29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="43" t="s">
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="36" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1771,17 +1757,17 @@
       <c r="B30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="46">
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="38">
         <v>14</v>
       </c>
     </row>
@@ -1790,17 +1776,17 @@
       <c r="B31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="37">
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="30">
         <v>6</v>
       </c>
     </row>
@@ -1809,17 +1795,17 @@
       <c r="B32" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="24"/>
-      <c r="L32" s="24"/>
-      <c r="M32" s="37" t="s">
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
+      <c r="K32" s="51"/>
+      <c r="L32" s="51"/>
+      <c r="M32" s="30" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1828,34 +1814,34 @@
       <c r="B33" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="24"/>
-      <c r="M33" s="31"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="24"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="24"/>
-      <c r="L34" s="24"/>
-      <c r="M34" s="37">
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="30">
         <v>12</v>
       </c>
     </row>
@@ -1864,34 +1850,34 @@
       <c r="B35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="24"/>
-      <c r="L35" s="24"/>
-      <c r="M35" s="44"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="24"/>
-      <c r="L36" s="24"/>
-      <c r="M36" s="37">
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="30">
         <v>23</v>
       </c>
     </row>
@@ -1900,34 +1886,34 @@
       <c r="B37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="24"/>
-      <c r="L37" s="24"/>
-      <c r="M37" s="31"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="24"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="32"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="25"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -1936,34 +1922,34 @@
       <c r="B39" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="30"/>
+      <c r="C39" s="48"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="48"/>
+      <c r="L39" s="48"/>
+      <c r="M39" s="23"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="32"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="49"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="25"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
@@ -1972,17 +1958,17 @@
       <c r="B41" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
-      <c r="I41" s="26"/>
-      <c r="J41" s="26"/>
-      <c r="K41" s="26"/>
-      <c r="L41" s="26"/>
-      <c r="M41" s="40"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="33"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
@@ -1991,17 +1977,17 @@
       <c r="B42" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="41"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="34"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
@@ -2010,68 +1996,68 @@
       <c r="B43" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="30"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="23"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24"/>
-      <c r="M44" s="31"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="51"/>
+      <c r="M44" s="24"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="31"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="51"/>
+      <c r="M45" s="24"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="32"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="25"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18" t="s">
@@ -2080,17 +2066,17 @@
       <c r="B47" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
-      <c r="K47" s="26"/>
-      <c r="L47" s="26"/>
-      <c r="M47" s="40"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="33"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
@@ -2099,34 +2085,34 @@
       <c r="B48" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="30"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="23"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="22"/>
-      <c r="M49" s="32"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="49"/>
+      <c r="M49" s="25"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -2135,34 +2121,34 @@
       <c r="B50" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="30"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="23"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="39" t="s">
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="49"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="32" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2173,72 +2159,72 @@
       <c r="B52" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="43" t="s">
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
+      <c r="E52" s="47"/>
+      <c r="F52" s="47"/>
+      <c r="G52" s="47"/>
+      <c r="H52" s="47"/>
+      <c r="I52" s="47"/>
+      <c r="J52" s="47"/>
+      <c r="K52" s="47"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="36" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="52" t="s">
+      <c r="A53" s="44" t="s">
         <v>86</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="30"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="J53" s="48"/>
+      <c r="K53" s="48"/>
+      <c r="L53" s="48"/>
+      <c r="M53" s="23"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="53"/>
+      <c r="A54" s="45"/>
       <c r="B54" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="31"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="24"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="54"/>
+      <c r="A55" s="46"/>
       <c r="B55" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="22"/>
-      <c r="M55" s="32"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="49"/>
+      <c r="M55" s="25"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
@@ -2253,34 +2239,34 @@
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="42"/>
+      <c r="M56" s="35"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M57" s="31"/>
+      <c r="M57" s="24"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M58" s="31"/>
+      <c r="M58" s="24"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M59" s="31"/>
+      <c r="M59" s="24"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M60" s="31"/>
+      <c r="M60" s="24"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M61" s="31"/>
+      <c r="M61" s="24"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M62" s="31"/>
+      <c r="M62" s="24"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M63" s="31"/>
+      <c r="M63" s="24"/>
     </row>
     <row r="65" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M65" s="31"/>
+      <c r="M65" s="24"/>
     </row>
     <row r="66" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M66" s="31"/>
+      <c r="M66" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>